<commit_message>
new csvs April 25
</commit_message>
<xml_diff>
--- a/status/excel/fromBox/BENT_excel.xlsx
+++ b/status/excel/fromBox/BENT_excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selenawallace/Library/Application Support/Box/Box Edit/Documents/1361512057765/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC7C30A-5ED5-9B46-9FDC-34865E59CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6DC7C30A-5ED5-9B46-9FDC-34865E59CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABA1A545-9794-4B48-9F95-513232F6AF3D}"/>
   <bookViews>
     <workbookView xWindow="12400" yWindow="500" windowWidth="16400" windowHeight="15840" xr2:uid="{6B535602-2BED-402B-BAD5-91FEE59FA3A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>index</t>
   </si>
@@ -81,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,17 +438,17 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.95">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -497,7 +497,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -514,35 +514,48 @@
         <v>45108</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45109</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>

</xml_diff>